<commit_message>
New index for excel data ouput, filtered nan (str) values to empty cells, table is sorted by hazopcase
</commit_message>
<xml_diff>
--- a/data/excel/PEA-HAZOP-Dosiermodul_v07.xlsx
+++ b/data/excel/PEA-HAZOP-Dosiermodul_v07.xlsx
@@ -536,35 +536,33 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Safeguard Otherinfo</t>
+          <t>Safeguard Other info</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Restrisiko Severity</t>
+          <t>Risk Graph Severity</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Restrisiko Frequency of Presence </t>
+          <t xml:space="preserve">Risk Graph Frequency of Presence </t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Restrisiko Possibility of avoiding</t>
+          <t>Risk Graph Possibility of avoiding</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Restrisiko Probability</t>
+          <t>Risk Graph Probability</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -573,7 +571,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Konzentration</t>
+          <t>Temperatur</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -583,7 +581,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>organisches Lösungsmittel</t>
+          <t>Überschreitung der zulässigen Temperatur im Behälter</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -593,17 +591,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Konzentration</t>
+          <t>Temperatur</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Mehr</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>organisches Lösungsmittel wird angeschlossen</t>
+          <t>Zugeführtes Prozessmedium zu heiß (&gt;200°C)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -611,24 +609,16 @@
           <t>Speicherbehälter</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Konzentration</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Mehr</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Beschädigung der Dichtungen</t>
+          <t>Materialversagen der Dichtungen, Leckage</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t xml:space="preserve">S3 - schwerwiegende </t>
+          <t>S2 - geringe</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -638,7 +628,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>G1 - möglich</t>
+          <t>G2 - fast unmöglich</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -648,24 +638,16 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>In 1 - Feed-Eingang</t>
+          <t>Speicherbehälter</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Schulung und SOPs</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Mitarbeiter vor Verwendung organischer Medien gut trainieren</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Hochwertige Dichtungen für Temp. über 200°C (bei 25bar)</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -673,7 +655,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>A1 - selten bis häufig</t>
+          <t>A2 - häufig bis andauernd</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -683,15 +665,13 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>W1 - sehr gering</t>
+          <t>W2 - gering</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -788,11 +768,7 @@
           <t>regelmäßige Prüfung des Sicherheitsventils (Ausbau + Test)</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -815,10 +791,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -827,7 +801,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Konzentration</t>
+          <t>Temperatur</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -837,47 +811,31 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>hohe Viskosität</t>
+          <t>Überschreitung der zulässigen Temperatur im Behälter</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>In 1 - Feed-Eingang</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Konzentration</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Mehr</t>
-        </is>
-      </c>
+          <t>Speicherbehälter</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>hoch viskoses Medium</t>
+          <t>Brand im Außenbereich, Strahlungswärme &gt;200°C</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Out 1 - Feed Ausgang</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Leistung</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Weniger</t>
-        </is>
-      </c>
+          <t>Speicherbehälter</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Pumpe ist überfordert</t>
+          <t>Leckage durch versagen der Dichtungen, Verdampfen der Edukte aufgrund hoher Umgebungstemperaturen</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -892,7 +850,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>G2 - fast unmöglich</t>
+          <t>G1 - möglich</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -902,37 +860,37 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>In 1 - Feed-Eingang</t>
+          <t>Speicherbehälter</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Schulung und SOPs</t>
+          <t>Stromlos-schalten des Moduls, Fail-safe stellung der Ventile</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Mitarbeiter vor Verwendung hoch-viskoser Medien gut trainieren</t>
+          <t xml:space="preserve">Brandmelde- und Löschanlage in Infrastruktur </t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>externe Sicherung notwendig</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t xml:space="preserve">S1 - minimale </t>
+          <t>S2 - geringe</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>A1 - selten bis häufig</t>
+          <t>A2 - häufig bis andauernd</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>G2 - fast unmöglich</t>
+          <t>G1 - möglich</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -942,10 +900,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -969,7 +925,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>In 2 - N2 Eingang</t>
+          <t>Speicherbehälter</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -984,7 +940,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Stoffverwechslung am Stickstoffeingang (z.B. Chlor)</t>
+          <t>Verunreinigung, bspw. Säure/Lauge die zu einer Wäremeentwicklung führen</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -994,17 +950,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Druck</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Mehr</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Bilden einer explosionsfähige Atmosphäre</t>
+          <t>Schlagartiges Verdampfen (Druckstoß) der Edukte aufgrund einer Reaktion im Behälter, bersten des Behälters</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -1024,32 +980,24 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>W1 - sehr gering</t>
+          <t>W2 - gering</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Speicherbehälter</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Organisatorisch ausschließen, dass Chlor an Inertisierung angeschlossen wird</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Sicherheitsventil VY3010</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr">
         <is>
-          <t xml:space="preserve">S3 - schwerwiegende </t>
+          <t xml:space="preserve">S1 - minimale </t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1064,15 +1012,13 @@
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>W1 - sehr gering</t>
+          <t>W2 - gering</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1081,37 +1027,37 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Konzentration</t>
+          <t>Temperatur</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Kein</t>
+          <t>Mehr</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>nur reines Lösungsmittel in Behälter</t>
+          <t>Überschreitung der zulässigen Temperatur im Behälter</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>In 1 - Feed-Eingang</t>
+          <t>In 2 - N2 Eingang</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Konzentration</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Kein</t>
+          <t>Anderer/Anders als</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>reines Lösungsmittel wird zugeführt</t>
+          <t>Stoffverwechslung am Stickstoffeingang (z.B. Chlor)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1119,24 +1065,16 @@
           <t>Speicherbehälter</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>kein</t>
+          <t>Bilden einer explosionsfähige Atmosphäre</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t xml:space="preserve">S1 - minimale </t>
+          <t xml:space="preserve">S3 - schwerwiegende </t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1151,55 +1089,41 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>W3 - relativ hoch</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>In 1 - Feed-Eingang</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>keine Aktion erforderlich</t>
-        </is>
-      </c>
+          <t>W1 - sehr gering</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Normalzustand</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Organisatorisch ausschließen, dass Chlor an Inertisierung angeschlossen wird</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">S3 - schwerwiegende </t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>A2 - häufig bis andauernd</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>G1 - möglich</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>W1 - sehr gering</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1208,62 +1132,54 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Konzentration</t>
+          <t>Temperatur</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>Weniger</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Unterschreitung der zulässigen Temperatur im Behälter</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Speicherbehälter</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Extrem niedrige Umgebungstemperatur</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Speicherbehälter</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Aggregatzustand</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>Anderer/Anders als</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Stickstoff zum Inertisieren</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>In 2 - N2 Eingang</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Konzentration</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Anderer/Anders als</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Luft, O2, CH4 oder andere brennbare Medien --&gt; HAZOPCase ID 5</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Speicherbehälter</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Druck</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Mehr</t>
-        </is>
-      </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Explosionsfähige Atmosphäre</t>
+          <t>Einfrieren des Mediums</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>S4 - katastophal</t>
+          <t>S2 - geringe</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1273,7 +1189,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>G2 - fast unmöglich</t>
+          <t>G1 - möglich</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1281,52 +1197,22 @@
           <t>W1 - sehr gering</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr">
         <is>
-          <t>Mitarbeiter vor Verwendung Stickstoff oder anderer gasförmiger Medien gut trainieren</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">S1 - minimale </t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>A1 - selten bis häufig</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>G2 - fast unmöglich</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>W1 - sehr gering</t>
-        </is>
-      </c>
+          <t>Betrieb nur im Innebereich bei moderaten Bedingungen</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1335,7 +1221,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Temperatur</t>
+          <t>Druck</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1345,27 +1231,27 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Überschreitung der zulässigen Temperatur im Behälter</t>
+          <t>Überschreitung des zulässigen Druckes im Behälter</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Speicherbehälter</t>
+          <t>In 1 - Feed-Eingang</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Druck</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Anderer/Anders als</t>
+          <t>Mehr</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Verunreinigung, bspw. Säure/Lauge die zu einer Wäremeentwicklung führen</t>
+          <t>Druck des eingehenden Mediums zu hoch</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1385,7 +1271,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Schlagartiges Verdampfen (Druckstoß) der Edukte aufgrund einer Reaktion im Behälter, bersten des Behälters</t>
+          <t>Druckerhöhung innerhalb des Behälters</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1418,16 +1304,8 @@
           <t>Sicherheitsventil VY3010</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -1450,10 +1328,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1462,7 +1338,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Temperatur</t>
+          <t>Druck</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1472,7 +1348,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Überschreitung der zulässigen Temperatur im Behälter</t>
+          <t>Überschreitung des zulässigen Druckes im Behälter</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1482,17 +1358,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Anderer/Anders als</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Brand im Außenbereich, Strahlungswärme &gt;200°C</t>
+          <t>Verunreinigung im Behälter führt zu exothermer Reaktion unter Gasbildung</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1502,22 +1378,22 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Druck</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Mehr</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Leckage durch versagen der Dichtungen, Verdampfen der Edukte aufgrund hoher Umgebungstemperaturen</t>
+          <t>Temperatur zusätzlich zum Druckanstieg im Behälter</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>S2 - geringe</t>
+          <t xml:space="preserve">S3 - schwerwiegende </t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1532,7 +1408,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>W1 - sehr gering</t>
+          <t>W2 - gering</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1542,22 +1418,14 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Stromlos-schalten des Moduls, Fail-safe stellung der Ventile</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Brandmelde- und Löschanlage in Infrastruktur </t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>externe Sicherung notwendig</t>
-        </is>
-      </c>
+          <t>Sicherheitsventil VY3010</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr">
         <is>
-          <t>S2 - geringe</t>
+          <t xml:space="preserve">S1 - minimale </t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1572,15 +1440,13 @@
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>W1 - sehr gering</t>
+          <t>W2 - gering</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A10" t="n">
+        <v>10</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1589,37 +1455,37 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Temperatur</t>
+          <t>Konzentration</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Weniger</t>
+          <t>Kein</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Unterschreitung der zulässigen Temperatur im Behälter</t>
+          <t>nur reines Lösungsmittel in Behälter</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Speicherbehälter</t>
+          <t>In 1 - Feed-Eingang</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Konzentration</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Kein</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Extrem niedrige Umgebungstemperatur</t>
+          <t>reines Lösungsmittel wird zugeführt</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1627,24 +1493,16 @@
           <t>Speicherbehälter</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Aggregatzustand</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Anderer/Anders als</t>
-        </is>
-      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Einfrieren des Mediums</t>
+          <t>kein</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>S2 - geringe</t>
+          <t xml:space="preserve">S1 - minimale </t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1659,55 +1517,33 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>W1 - sehr gering</t>
+          <t>W3 - relativ hoch</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>In 1 - Feed-Eingang</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>keine Aktion erforderlich</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>Betrieb nur im Innebereich bei moderaten Bedingungen</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Normalzustand</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A11" t="n">
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1716,7 +1552,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Temperatur</t>
+          <t>Konzentration</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1726,7 +1562,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Überschreitung der zulässigen Temperatur im Behälter</t>
+          <t>starke Säure oder Base</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1736,7 +1572,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Temperatur</t>
+          <t>Konzentration</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1746,7 +1582,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Zugeführtes Prozessmedium zu heiß (&gt;200°C)</t>
+          <t>starke Säure oder Base wird zugeführt</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1756,22 +1592,22 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Konzentration</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Mehr</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Materialversagen der Dichtungen, Leckage</t>
+          <t>Korrosion an Wand, Schweißnähte oder Dichtungen</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>S2 - geringe</t>
+          <t>S4 - katastophal</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1786,29 +1622,25 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>W2 - gering</t>
+          <t>W1 - sehr gering</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>Speicherbehälter</t>
+          <t>In 1 - Feed-Eingang</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Hochwertige Dichtungen für Temp. über 200°C (bei 25bar)</t>
+          <t>Schulung und SOPs</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Mitarbeiter vor Verwendung starker Säuren und Basen gut trainieren</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -1816,7 +1648,7 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>A2 - häufig bis andauernd</t>
+          <t>A1 - selten bis häufig</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
@@ -1826,15 +1658,13 @@
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>W2 - gering</t>
+          <t>W1 - sehr gering</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="A12" t="n">
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1853,12 +1683,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dichtungsabrieb in Behälter </t>
+          <t>organisches Lösungsmittel</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Speicherbehälter</t>
+          <t>In 1 - Feed-Eingang</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1866,39 +1696,35 @@
           <t>Konzentration</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Mehr</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Feststoffe gelangen in Behälter</t>
+          <t>organisches Lösungsmittel wird angeschlossen</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Out 1 - Feed Ausgang</t>
+          <t>Speicherbehälter</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Druck</t>
+          <t>Konzentration</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Weniger</t>
+          <t>Mehr</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Höherer Druckverlust über Filter, Pumpe kavitiert</t>
+          <t>Beschädigung der Dichtungen</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>S2 - geringe</t>
+          <t xml:space="preserve">S3 - schwerwiegende </t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
@@ -1918,24 +1744,20 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>In 1 - Feed-Eingang</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Schulung und SOPs</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>MA überprüfen vor jedem Befüllen die Behälterdichtungen</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Mitarbeiter vor Verwendung organischer Medien gut trainieren</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -1958,10 +1780,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A13" t="n">
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1980,7 +1800,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>starke Säure oder Base</t>
+          <t>hohe Viskosität</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -2000,32 +1820,32 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>starke Säure oder Base wird zugeführt</t>
+          <t>hoch viskoses Medium</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Speicherbehälter</t>
+          <t>Out 1 - Feed Ausgang</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Konzentration</t>
+          <t>Leistung</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Mehr</t>
+          <t>Weniger</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Korrosion an Wand, Schweißnähte oder Dichtungen</t>
+          <t>Pumpe ist überfordert</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>S4 - katastophal</t>
+          <t>S2 - geringe</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
@@ -2055,14 +1875,10 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>Mitarbeiter vor Verwendung starker Säuren und Basen gut trainieren</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Mitarbeiter vor Verwendung hoch-viskoser Medien gut trainieren</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -2085,10 +1901,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A14" t="n">
+        <v>14</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -2097,62 +1911,62 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Konzentration</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Mehr</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Feststoffe bilden sich</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Speicherbehälter</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Konzentration</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Mehr</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Feststoffe durch Überschreiten einer Sättigungskonszentration</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Out 1 - Feed Ausgang</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
           <t>Druck</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Mehr</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Überschreitung des zulässigen Druckes im Behälter</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>In 1 - Feed-Eingang</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Druck</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Mehr</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Druck des eingehenden Mediums zu hoch</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Speicherbehälter</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Druck</t>
-        </is>
-      </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Mehr</t>
+          <t>Weniger</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Druckerhöhung innerhalb des Behälters</t>
+          <t>Höherer Druckverlust über Filter, Pumpe kavitiert</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t xml:space="preserve">S3 - schwerwiegende </t>
+          <t>S2 - geringe</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
@@ -2170,26 +1984,14 @@
           <t>W2 - gering</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>Speicherbehälter</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Sicherheitsventil VY3010</t>
-        </is>
-      </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Bei häufigem Feststoffauftritt muss Filter wechselbar sein, bzw. Parallelen Filter oder Bypass-Schaltung für Filter FL1010</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -2197,25 +1999,23 @@
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>A2 - häufig bis andauernd</t>
+          <t>A1 - selten bis häufig</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>G1 - möglich</t>
+          <t>G2 - fast unmöglich</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>W2 - gering</t>
+          <t>W1 - sehr gering</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A15" t="n">
+        <v>15</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -2312,11 +2112,7 @@
           <t>Filter muss bei Feststoffgefahr am Einlass vorgesehen werden, oder MA werden auf Vorhandensein von Feststoffen geschult</t>
         </is>
       </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -2339,10 +2135,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A16" t="n">
+        <v>16</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -2351,62 +2145,62 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>Konzentration</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Mehr</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dichtungsabrieb in Behälter </t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Speicherbehälter</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Konzentration</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Mehr</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Feststoffe gelangen in Behälter</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Out 1 - Feed Ausgang</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
           <t>Druck</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Mehr</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Überschreitung des zulässigen Druckes im Behälter</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Speicherbehälter</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Anderer/Anders als</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Verunreinigung im Behälter führt zu exothermer Reaktion unter Gasbildung</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Speicherbehälter</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Druck</t>
-        </is>
-      </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Mehr</t>
+          <t>Weniger</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Temperatur zusätzlich zum Druckanstieg im Behälter</t>
+          <t>Höherer Druckverlust über Filter, Pumpe kavitiert</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t xml:space="preserve">S3 - schwerwiegende </t>
+          <t>S2 - geringe</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -2424,26 +2218,14 @@
           <t>W2 - gering</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>Speicherbehälter</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>Sicherheitsventil VY3010</t>
-        </is>
-      </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>MA überprüfen vor jedem Befüllen die Behälterdichtungen</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>
@@ -2451,25 +2233,23 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>A2 - häufig bis andauernd</t>
+          <t>A1 - selten bis häufig</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>G1 - möglich</t>
+          <t>G2 - fast unmöglich</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>W2 - gering</t>
+          <t>W1 - sehr gering</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="A17" t="n">
+        <v>17</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -2483,17 +2263,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Mehr</t>
+          <t>Anderer/Anders als</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Feststoffe bilden sich</t>
+          <t>Stickstoff zum Inertisieren</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Speicherbehälter</t>
+          <t>In 2 - N2 Eingang</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2503,17 +2283,17 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Mehr</t>
+          <t>Anderer/Anders als</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Feststoffe durch Überschreiten einer Sättigungskonszentration</t>
+          <t>Luft, O2, CH4 oder andere brennbare Medien --&gt; HAZOPCase ID 5</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Out 1 - Feed Ausgang</t>
+          <t>Speicherbehälter</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -2523,17 +2303,17 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Weniger</t>
+          <t>Mehr</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Höherer Druckverlust über Filter, Pumpe kavitiert</t>
+          <t>Explosionsfähige Atmosphäre</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>S2 - geringe</t>
+          <t>S4 - katastophal</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -2543,34 +2323,22 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>G1 - möglich</t>
+          <t>G2 - fast unmöglich</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>W2 - gering</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>W1 - sehr gering</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr">
         <is>
-          <t>Bei häufigem Feststoffauftritt muss Filter wechselbar sein, bzw. Parallelen Filter oder Bypass-Schaltung für Filter FL1010</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>Mitarbeiter vor Verwendung Stickstoff oder anderer gasförmiger Medien gut trainieren</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr">
         <is>
           <t xml:space="preserve">S1 - minimale </t>

</xml_diff>

<commit_message>
Docs: sequence diagrams update
</commit_message>
<xml_diff>
--- a/data/excel/PEA-HAZOP-Dosiermodul_v07.xlsx
+++ b/data/excel/PEA-HAZOP-Dosiermodul_v07.xlsx
@@ -587,7 +587,7 @@
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Frequency of Presence </t>
+          <t>Frequency of Presence</t>
         </is>
       </c>
       <c r="Q2" s="1" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="X2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Frequency of Presence </t>
+          <t>Frequency of Presence</t>
         </is>
       </c>
       <c r="Y2" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Graph ontology: improved RDF Graph schema
-added clear subject, blanknode and predicate urirefs for all data members
-adopted sparql query

Config
-renamed some header
</commit_message>
<xml_diff>
--- a/data/excel/PEA-HAZOP-Dosiermodul_v07.xlsx
+++ b/data/excel/PEA-HAZOP-Dosiermodul_v07.xlsx
@@ -517,7 +517,7 @@
       <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>ID HAZOP Case</t>
+          <t>HAZOP Case ID</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -587,7 +587,7 @@
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t>Frequency of Presence</t>
+          <t>Frequency of presence</t>
         </is>
       </c>
       <c r="Q2" s="1" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="X2" s="1" t="inlineStr">
         <is>
-          <t>Frequency of Presence</t>
+          <t>Frequency of presence</t>
         </is>
       </c>
       <c r="Y2" s="1" t="inlineStr">

</xml_diff>